<commit_message>
Update pages, code, data for LA pages
</commit_message>
<xml_diff>
--- a/data/source/recent/lasd_compstat.xlsx
+++ b/data/source/recent/lasd_compstat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Jarvis/R/safetytracker_losangeles/data/source/recent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541AD4C5-AFE1-6745-9FB8-64AE79697199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9979FD89-92CF-FF4C-A83F-4D9E5C23475A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36360" yWindow="500" windowWidth="18340" windowHeight="17420" xr2:uid="{62D3A5B9-DFAB-2342-B627-2572A7BF831A}"/>
+    <workbookView xWindow="39100" yWindow="4440" windowWidth="18340" windowHeight="17420" xr2:uid="{62D3A5B9-DFAB-2342-B627-2572A7BF831A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,6 @@
     <t>Malibu/Lost Hills</t>
   </si>
   <si>
-    <t>Marina del Ray</t>
-  </si>
-  <si>
     <t>Norwalk</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Walnut/Diamond Bar</t>
+  </si>
+  <si>
+    <t>Marina Del Rey</t>
   </si>
 </sst>
 </file>
@@ -510,8 +510,8 @@
   <dimension ref="A1:H169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B146" sqref="B146"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,33 +523,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
       <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
       <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
         <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
         <v>12</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>12</v>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
         <v>12</v>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
         <v>12</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
         <v>13</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
         <v>13</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
@@ -1719,7 +1719,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
         <v>13</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B52" t="s">
         <v>14</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B53" t="s">
         <v>14</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" t="s">
         <v>14</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B55" t="s">
         <v>14</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B56" t="s">
         <v>14</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B57" t="s">
         <v>14</v>
@@ -2005,7 +2005,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B58" t="s">
         <v>15</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
@@ -2057,7 +2057,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B61" t="s">
         <v>15</v>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B62" t="s">
         <v>15</v>
@@ -2135,7 +2135,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B63" t="s">
         <v>15</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B64" t="s">
         <v>15</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B65" t="s">
         <v>16</v>
@@ -2213,7 +2213,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B66" t="s">
         <v>16</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B67" t="s">
         <v>16</v>
@@ -2265,7 +2265,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B68" t="s">
         <v>16</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B69" t="s">
         <v>16</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B70" t="s">
         <v>16</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B71" t="s">
         <v>16</v>
@@ -2369,7 +2369,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B72" t="s">
         <v>17</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B73" t="s">
         <v>17</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B74" t="s">
         <v>17</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B75" t="s">
         <v>17</v>
@@ -2473,7 +2473,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B76" t="s">
         <v>17</v>
@@ -2499,7 +2499,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B77" t="s">
         <v>17</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B78" t="s">
         <v>17</v>
@@ -2551,7 +2551,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B79" t="s">
         <v>18</v>
@@ -2577,7 +2577,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B80" t="s">
         <v>18</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B81" t="s">
         <v>18</v>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B82" t="s">
         <v>18</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B83" t="s">
         <v>18</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B84" t="s">
         <v>18</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B85" t="s">
         <v>18</v>
@@ -2733,7 +2733,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B86" t="s">
         <v>19</v>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B87" t="s">
         <v>19</v>
@@ -2785,7 +2785,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B88" t="s">
         <v>19</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B89" t="s">
         <v>19</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B90" t="s">
         <v>19</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B91" t="s">
         <v>19</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B92" t="s">
         <v>19</v>
@@ -2915,10 +2915,10 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B93" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C93" t="s">
         <v>2</v>
@@ -2941,10 +2941,10 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C94" t="s">
         <v>3</v>
@@ -2967,10 +2967,10 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B95" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C95" t="s">
         <v>4</v>
@@ -2993,10 +2993,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B96" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
@@ -3019,10 +3019,10 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B97" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
@@ -3045,10 +3045,10 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B98" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C98" t="s">
         <v>7</v>
@@ -3071,10 +3071,10 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B99" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -3097,10 +3097,10 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B100" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C100" t="s">
         <v>2</v>
@@ -3123,10 +3123,10 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B101" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C101" t="s">
         <v>3</v>
@@ -3149,10 +3149,10 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B102" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C102" t="s">
         <v>4</v>
@@ -3175,10 +3175,10 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B103" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C103" t="s">
         <v>5</v>
@@ -3201,10 +3201,10 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B104" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C104" t="s">
         <v>6</v>
@@ -3227,10 +3227,10 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B105" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C105" t="s">
         <v>7</v>
@@ -3253,10 +3253,10 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B106" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -3279,10 +3279,10 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B107" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C107" t="s">
         <v>2</v>
@@ -3305,10 +3305,10 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B108" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C108" t="s">
         <v>3</v>
@@ -3331,10 +3331,10 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B109" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C109" t="s">
         <v>4</v>
@@ -3357,10 +3357,10 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B110" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C110" t="s">
         <v>5</v>
@@ -3383,10 +3383,10 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B111" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
@@ -3409,10 +3409,10 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B112" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C112" t="s">
         <v>7</v>
@@ -3435,10 +3435,10 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B113" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -3461,10 +3461,10 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B114" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C114" t="s">
         <v>2</v>
@@ -3487,10 +3487,10 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B115" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C115" t="s">
         <v>3</v>
@@ -3513,10 +3513,10 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B116" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C116" t="s">
         <v>4</v>
@@ -3539,10 +3539,10 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B117" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C117" t="s">
         <v>5</v>
@@ -3565,10 +3565,10 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B118" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C118" t="s">
         <v>6</v>
@@ -3591,10 +3591,10 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B119" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C119" t="s">
         <v>7</v>
@@ -3617,10 +3617,10 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B120" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -3643,10 +3643,10 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B121" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C121" t="s">
         <v>2</v>
@@ -3669,10 +3669,10 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B122" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C122" t="s">
         <v>3</v>
@@ -3695,10 +3695,10 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B123" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C123" t="s">
         <v>4</v>
@@ -3721,10 +3721,10 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B124" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C124" t="s">
         <v>5</v>
@@ -3747,10 +3747,10 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B125" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C125" t="s">
         <v>6</v>
@@ -3773,10 +3773,10 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B126" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C126" t="s">
         <v>7</v>
@@ -3799,10 +3799,10 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B127" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -3825,10 +3825,10 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B128" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C128" t="s">
         <v>2</v>
@@ -3851,10 +3851,10 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C129" t="s">
         <v>3</v>
@@ -3877,10 +3877,10 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B130" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C130" t="s">
         <v>4</v>
@@ -3903,10 +3903,10 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B131" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
@@ -3929,10 +3929,10 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B132" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
@@ -3955,10 +3955,10 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B133" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C133" t="s">
         <v>7</v>
@@ -3981,10 +3981,10 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B134" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -4007,10 +4007,10 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B135" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C135" t="s">
         <v>2</v>
@@ -4033,10 +4033,10 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B136" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C136" t="s">
         <v>3</v>
@@ -4059,10 +4059,10 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B137" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C137" t="s">
         <v>4</v>
@@ -4085,10 +4085,10 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B138" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C138" t="s">
         <v>5</v>
@@ -4111,10 +4111,10 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B139" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C139" t="s">
         <v>6</v>
@@ -4137,10 +4137,10 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B140" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C140" t="s">
         <v>7</v>
@@ -4163,10 +4163,10 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B141" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -4189,10 +4189,10 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B142" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C142" t="s">
         <v>2</v>
@@ -4215,10 +4215,10 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B143" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C143" t="s">
         <v>3</v>
@@ -4241,10 +4241,10 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B144" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C144" t="s">
         <v>4</v>
@@ -4267,10 +4267,10 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B145" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C145" t="s">
         <v>5</v>
@@ -4293,10 +4293,10 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B146" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C146" t="s">
         <v>6</v>
@@ -4319,10 +4319,10 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B147" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C147" t="s">
         <v>7</v>
@@ -4345,10 +4345,10 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B148" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
@@ -4371,10 +4371,10 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B149" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C149" t="s">
         <v>2</v>
@@ -4397,10 +4397,10 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B150" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C150" t="s">
         <v>3</v>
@@ -4423,10 +4423,10 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B151" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C151" t="s">
         <v>4</v>
@@ -4449,10 +4449,10 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B152" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C152" t="s">
         <v>5</v>
@@ -4475,10 +4475,10 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B153" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C153" t="s">
         <v>6</v>
@@ -4501,10 +4501,10 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B154" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C154" t="s">
         <v>7</v>
@@ -4527,10 +4527,10 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B155" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C155" t="s">
         <v>8</v>
@@ -4553,10 +4553,10 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B156" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C156" t="s">
         <v>2</v>
@@ -4579,10 +4579,10 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B157" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C157" t="s">
         <v>3</v>
@@ -4605,10 +4605,10 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B158" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C158" t="s">
         <v>4</v>
@@ -4631,10 +4631,10 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B159" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C159" t="s">
         <v>5</v>
@@ -4657,10 +4657,10 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B160" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C160" t="s">
         <v>6</v>
@@ -4683,10 +4683,10 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B161" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C161" t="s">
         <v>7</v>
@@ -4709,10 +4709,10 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B162" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C162" t="s">
         <v>8</v>
@@ -4735,10 +4735,10 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>36</v>
+      </c>
+      <c r="B163" t="s">
         <v>37</v>
-      </c>
-      <c r="B163" t="s">
-        <v>38</v>
       </c>
       <c r="C163" t="s">
         <v>2</v>
@@ -4761,10 +4761,10 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>36</v>
+      </c>
+      <c r="B164" t="s">
         <v>37</v>
-      </c>
-      <c r="B164" t="s">
-        <v>38</v>
       </c>
       <c r="C164" t="s">
         <v>3</v>
@@ -4787,10 +4787,10 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>36</v>
+      </c>
+      <c r="B165" t="s">
         <v>37</v>
-      </c>
-      <c r="B165" t="s">
-        <v>38</v>
       </c>
       <c r="C165" t="s">
         <v>4</v>
@@ -4813,10 +4813,10 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>36</v>
+      </c>
+      <c r="B166" t="s">
         <v>37</v>
-      </c>
-      <c r="B166" t="s">
-        <v>38</v>
       </c>
       <c r="C166" t="s">
         <v>5</v>
@@ -4839,10 +4839,10 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>36</v>
+      </c>
+      <c r="B167" t="s">
         <v>37</v>
-      </c>
-      <c r="B167" t="s">
-        <v>38</v>
       </c>
       <c r="C167" t="s">
         <v>6</v>
@@ -4865,10 +4865,10 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>36</v>
+      </c>
+      <c r="B168" t="s">
         <v>37</v>
-      </c>
-      <c r="B168" t="s">
-        <v>38</v>
       </c>
       <c r="C168" t="s">
         <v>7</v>
@@ -4891,10 +4891,10 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>36</v>
+      </c>
+      <c r="B169" t="s">
         <v>37</v>
-      </c>
-      <c r="B169" t="s">
-        <v>38</v>
       </c>
       <c r="C169" t="s">
         <v>8</v>

</xml_diff>